<commit_message>
reorganisation dossier: creation dossier backend pour le server
</commit_message>
<xml_diff>
--- a/Projet/Template+de+Plan+de+tests.xlsx
+++ b/Projet/Template+de+Plan+de+tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggira\Desktop\site\lab\Orinoco\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD089D27-55DB-4756-A5FA-E38ECDFACFD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B98D37-AC18-481E-A345-4CD684C02134}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="630" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan test modele" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="115">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -346,20 +346,6 @@
 afficher le nombre d'article sur l'icone de l'accueil</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">supprimer un produit du </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">tableau panier </t>
-    </r>
-  </si>
-  <si>
     <t>controleFormulaire</t>
   </si>
   <si>
@@ -398,9 +384,6 @@
 ALORS envoieDonneesApi</t>
   </si>
   <si>
-    <t>ajoutNouveauProduit</t>
-  </si>
-  <si>
     <t>compteurNombreProduit</t>
   </si>
   <si>
@@ -408,10 +391,6 @@
   </si>
   <si>
     <t>getDonneesApiPersonnalisation</t>
-  </si>
-  <si>
-    <t>retourner les strings
-correspondant aux options de personnalisation de chaque type de produit</t>
   </si>
   <si>
     <t>personnalisationProduitHTML</t>
@@ -424,37 +403,12 @@
 stringTableauPanier</t>
   </si>
   <si>
-    <t>Convertir les donnes du array en string</t>
-  </si>
-  <si>
     <t>Recuperer les informations de tous les éléments
 prends en parametre l'URL pour la dupliquer facilement a chaque catégorie
 Utiliser les promesses ici</t>
   </si>
   <si>
     <t>onreadystatechange</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A chaque ajout d'un contenu au </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>tableau panier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, ajout d'une nouvelle ligne avec la descritpion du produit</t>
-    </r>
   </si>
   <si>
     <r>
@@ -477,8 +431,66 @@
     <t>POUR CHAQUE index present dans le tableau, CRÉER un nouveau bloc produit HTML qui contiendra le contenu de la description du produit</t>
   </si>
   <si>
-    <t>CRÉER un nouveau bloc element produit en html qui retourne les elements descriptif du produit
-Attribut a chaque nouveau bloc avec un numéro</t>
+    <t>console.log pour verifier que le nombre de bloc correspond à la numérotation</t>
+  </si>
+  <si>
+    <t>tableauProduitPanier</t>
+  </si>
+  <si>
+    <t>CRÉER un tableau de produit panier. Ajout du produit EN FONCTION de son ID</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A chaque ajout d'un contenu au </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>tableauProduitPanier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, ajout d'une nouvelle ligne avec la description du produit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">supprimer un produit du </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">tableau panier </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+modif de quantité</t>
+    </r>
+  </si>
+  <si>
+    <t>Convertir les donnes du array en string
+A REECRIRE</t>
+  </si>
+  <si>
+    <t>Fonction generique avec la 1ere fonction de recuperation IF id present 
+REFLEXION AVEC UNE FONCTION GLOBALE DE REQUETE</t>
   </si>
 </sst>
 </file>
@@ -540,7 +552,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,6 +580,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -657,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -699,6 +717,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,8 +954,8 @@
   <dimension ref="A1:Z1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -983,7 +1017,7 @@
         <v>74</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -994,10 +1028,10 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1011,7 +1045,7 @@
         <v>76</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -1022,38 +1056,40 @@
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" s="12"/>
+        <v>99</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:26" s="23" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>75</v>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>85</v>
+        <v>100</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -1064,58 +1100,58 @@
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="14" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="15" t="s">
-        <v>97</v>
+      <c r="C10" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+        <v>111</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="11"/>
-      <c r="C11" s="14" t="s">
-        <v>79</v>
+      <c r="C11" s="15" t="s">
+        <v>96</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+        <v>80</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="16" t="s">
         <v>78</v>
       </c>
       <c r="B12" s="11"/>
@@ -1143,15 +1179,15 @@
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="25" t="s">
         <v>78</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -1162,10 +1198,10 @@
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
@@ -1175,11 +1211,11 @@
         <v>78</v>
       </c>
       <c r="B16" s="11"/>
-      <c r="C16" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>107</v>
+      <c r="C16" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>113</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="12"/>
@@ -1190,10 +1226,10 @@
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="12"/>
@@ -1204,24 +1240,24 @@
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>

</xml_diff>

<commit_message>
test utilisation des promesses
</commit_message>
<xml_diff>
--- a/Projet/Template+de+Plan+de+tests.xlsx
+++ b/Projet/Template+de+Plan+de+tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggira\Desktop\site\lab\Orinoco\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B98D37-AC18-481E-A345-4CD684C02134}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6786CB-FAB4-4817-BF79-FB30CF6C2132}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="112">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -336,12 +336,6 @@
     <t>Calculer le prix totale suivant le nombre d'article ajouté</t>
   </si>
   <si>
-    <t>barreRechercherProduit</t>
-  </si>
-  <si>
-    <t>afficher les produits ayant les valeurs dans la barre de recherche</t>
-  </si>
-  <si>
     <t>compter le nombre d'article dans le panier
 afficher le nombre d'article sur l'icone de l'accueil</t>
   </si>
@@ -384,19 +378,10 @@
 ALORS envoieDonneesApi</t>
   </si>
   <si>
-    <t>compteurNombreProduit</t>
-  </si>
-  <si>
-    <t>compte le nombre de bloc de produit en html</t>
-  </si>
-  <si>
     <t>getDonneesApiPersonnalisation</t>
   </si>
   <si>
     <t>personnalisationProduitHTML</t>
-  </si>
-  <si>
-    <t>la fonction doit ajouter la personnalisation sur le html</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -426,12 +411,6 @@
       </rPr>
       <t>tableauDonnees</t>
     </r>
-  </si>
-  <si>
-    <t>POUR CHAQUE index present dans le tableau, CRÉER un nouveau bloc produit HTML qui contiendra le contenu de la description du produit</t>
-  </si>
-  <si>
-    <t>console.log pour verifier que le nombre de bloc correspond à la numérotation</t>
   </si>
   <si>
     <t>tableauProduitPanier</t>
@@ -491,6 +470,19 @@
   <si>
     <t>Fonction generique avec la 1ere fonction de recuperation IF id present 
 REFLEXION AVEC UNE FONCTION GLOBALE DE REQUETE</t>
+  </si>
+  <si>
+    <t>la fonction doit ajouter la personnalisation dans le html</t>
+  </si>
+  <si>
+    <t>POUR CHAQUE index present dans le tableau, AJOUTER un nouveau bloc HTML qui contiendra le contenu de la description du produit</t>
+  </si>
+  <si>
+    <t>clickEnvoiePageProduit</t>
+  </si>
+  <si>
+    <t>Au click sur le produit, ouvre une nouvelle page,
+RETOURNE les informations du produit concerné dans le HTML de la page produit</t>
   </si>
 </sst>
 </file>
@@ -552,7 +544,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,12 +560,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -675,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -716,22 +702,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,11 +930,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1005"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1009,7 +988,7 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="5"/>
@@ -1017,21 +996,21 @@
         <v>74</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>75</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1045,40 +1024,38 @@
         <v>76</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
-        <v>75</v>
+    <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>108</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:26" s="23" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
+    <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -1086,24 +1063,24 @@
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>114</v>
+        <v>97</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
@@ -1114,80 +1091,80 @@
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="14" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+        <v>104</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="B11" s="11"/>
-      <c r="C11" s="15" t="s">
-        <v>96</v>
+      <c r="C11" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="19" t="s">
         <v>78</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="14" t="s">
-        <v>82</v>
+      <c r="C13" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="15" t="s">
-        <v>95</v>
+      <c r="C14" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -1197,13 +1174,13 @@
         <v>78</v>
       </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="12"/>
+      <c r="C15" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="4"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1211,11 +1188,11 @@
         <v>78</v>
       </c>
       <c r="B16" s="11"/>
-      <c r="C16" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>113</v>
+      <c r="C16" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="12"/>
@@ -1225,70 +1202,63 @@
         <v>78</v>
       </c>
       <c r="B17" s="11"/>
-      <c r="C17" s="15" t="s">
-        <v>94</v>
+      <c r="C17" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E17" s="4"/>
+        <v>91</v>
+      </c>
+      <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>89</v>
-      </c>
+    <row r="19" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
       <c r="B19" s="11"/>
-      <c r="C19" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="12"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
-      <c r="B20" s="11"/>
+      <c r="B20" s="3"/>
       <c r="C20" s="11"/>
       <c r="D20" s="12"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
       <c r="E21" s="12"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
@@ -1306,7 +1276,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
@@ -1412,11 +1382,9 @@
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
     </row>
     <row r="42" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D42" s="2"/>
@@ -1463,7 +1431,7 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
@@ -6232,11 +6200,6 @@
       <c r="D1004" s="2"/>
       <c r="E1004" s="2"/>
       <c r="F1004" s="2"/>
-    </row>
-    <row r="1005" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D1005" s="2"/>
-      <c r="E1005" s="2"/>
-      <c r="F1005" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test lien js accueil vers produit
</commit_message>
<xml_diff>
--- a/Projet/Template+de+Plan+de+tests.xlsx
+++ b/Projet/Template+de+Plan+de+tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggira\Desktop\site\lab\Orinoco\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6786CB-FAB4-4817-BF79-FB30CF6C2132}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40614321-1169-409F-A069-EA12F05F6BF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="630" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan test modele" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="113">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -484,6 +484,9 @@
     <t>Au click sur le produit, ouvre une nouvelle page,
 RETOURNE les informations du produit concerné dans le HTML de la page produit</t>
   </si>
+  <si>
+    <t>au click, si l'ID du lien est egale a un Id du tableau, ALORS je recupere le lien URL de l'article correspondant</t>
+  </si>
 </sst>
 </file>
 
@@ -932,9 +935,9 @@
   </sheetPr>
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1026,7 +1029,9 @@
       <c r="D4" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
integration bootstrap et 1ere mise en forme de bloc
</commit_message>
<xml_diff>
--- a/Projet/Template+de+Plan+de+tests.xlsx
+++ b/Projet/Template+de+Plan+de+tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggira\Desktop\site\lab\Orinoco\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40614321-1169-409F-A069-EA12F05F6BF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295C7DFE-D6E9-4230-B32E-6C07949FAEBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="630" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan test modele" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="121">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -290,9 +290,6 @@
   </si>
   <si>
     <t>accueil js</t>
-  </si>
-  <si>
-    <t>descriptionProduitHTML</t>
   </si>
   <si>
     <t>produit js</t>
@@ -388,29 +385,7 @@
 stringTableauPanier</t>
   </si>
   <si>
-    <t>Recuperer les informations de tous les éléments
-prends en parametre l'URL pour la dupliquer facilement a chaque catégorie
-Utiliser les promesses ici</t>
-  </si>
-  <si>
     <t>onreadystatechange</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">recupere les donnees de l'API, elles sont stocké sous la forme d'un tableau, avec pour chaque index = un produit.
-Chaque index contient des objets correspondant a la description des produits
-Ce tableau est le </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>tableauDonnees</t>
-    </r>
   </si>
   <si>
     <t>tableauProduitPanier</t>
@@ -475,24 +450,59 @@
     <t>la fonction doit ajouter la personnalisation dans le html</t>
   </si>
   <si>
-    <t>POUR CHAQUE index present dans le tableau, AJOUTER un nouveau bloc HTML qui contiendra le contenu de la description du produit</t>
-  </si>
-  <si>
-    <t>clickEnvoiePageProduit</t>
-  </si>
-  <si>
-    <t>Au click sur le produit, ouvre une nouvelle page,
-RETOURNE les informations du produit concerné dans le HTML de la page produit</t>
-  </si>
-  <si>
-    <t>au click, si l'ID du lien est egale a un Id du tableau, ALORS je recupere le lien URL de l'article correspondant</t>
+    <t>listeProduitsAccueil</t>
+  </si>
+  <si>
+    <t>Recuperer les donnees de l'API, à partir de l'ID correspondant ,
+Intégration du contenu dans le HTML</t>
+  </si>
+  <si>
+    <t>getPromise</t>
+  </si>
+  <si>
+    <t>Recupere les donnees de la promesse pour les retourner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">envoie la requete au serveur </t>
+  </si>
+  <si>
+    <t>getPromise().then</t>
+  </si>
+  <si>
+    <t>Une fois les getPromise retournée, je peux utiliser les donnees</t>
+  </si>
+  <si>
+    <t>creationBlocHtmlProduit</t>
+  </si>
+  <si>
+    <t>creation du bloc html pour la page produit</t>
+  </si>
+  <si>
+    <t>creationBlocHTMLAccueil</t>
+  </si>
+  <si>
+    <t>creation du bloc html pour la page accueil</t>
+  </si>
+  <si>
+    <t>POUR CHAQUE index present dans le tableau, AJOUTER les parametres a la fonction creationBlocHTMLAccueil</t>
+  </si>
+  <si>
+    <t>insertionDescriptifProduits</t>
+  </si>
+  <si>
+    <t>accueil js
+porduit js</t>
+  </si>
+  <si>
+    <t>Creation de la fonction promesse qui prend en parametre l'URL et retourne la promesse
+pour la page produit, ajout d'un parametre à l'URL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -536,13 +546,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0070C0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -664,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -714,6 +717,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -933,11 +940,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -991,318 +998,344 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>75</v>
+      <c r="A2" s="23" t="s">
+        <v>119</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
         <v>74</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>75</v>
+      <c r="A3" s="23" t="s">
+        <v>119</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="14" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" s="18" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>80</v>
+      <c r="C10" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>104</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>78</v>
+      <c r="A11" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="14" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="14" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="14" t="s">
-        <v>85</v>
+      <c r="C14" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>78</v>
+      <c r="A15" s="16" t="s">
+        <v>77</v>
       </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="E15" s="4"/>
+      <c r="C15" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="11"/>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="14" t="s">
-        <v>90</v>
-      </c>
       <c r="D17" s="4" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
+    <row r="19" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
+      <c r="C19" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>103</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
+    <row r="20" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="3"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
+    <row r="22" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="4"/>
@@ -1387,24 +1420,32 @@
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
     </row>
     <row r="42" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
     </row>
     <row r="44" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
     </row>
     <row r="45" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D45" s="2"/>
@@ -1436,22 +1477,22 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
@@ -6205,6 +6246,26 @@
       <c r="D1004" s="2"/>
       <c r="E1004" s="2"/>
       <c r="F1004" s="2"/>
+    </row>
+    <row r="1005" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1005" s="2"/>
+      <c r="E1005" s="2"/>
+      <c r="F1005" s="2"/>
+    </row>
+    <row r="1006" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1006" s="2"/>
+      <c r="E1006" s="2"/>
+      <c r="F1006" s="2"/>
+    </row>
+    <row r="1007" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1007" s="2"/>
+      <c r="E1007" s="2"/>
+      <c r="F1007" s="2"/>
+    </row>
+    <row r="1008" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1008" s="2"/>
+      <c r="E1008" s="2"/>
+      <c r="F1008" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
essaie de recuperation avec fectch
</commit_message>
<xml_diff>
--- a/Projet/Template+de+Plan+de+tests.xlsx
+++ b/Projet/Template+de+Plan+de+tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggira\Desktop\site\lab\Orinoco\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295C7DFE-D6E9-4230-B32E-6C07949FAEBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6790F36-7F3F-4E6B-917D-3AAED3C9218E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan test modele" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="126">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -375,12 +375,6 @@
 ALORS envoieDonneesApi</t>
   </si>
   <si>
-    <t>getDonneesApiPersonnalisation</t>
-  </si>
-  <si>
-    <t>personnalisationProduitHTML</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 stringTableauPanier</t>
   </si>
@@ -443,13 +437,6 @@
 A REECRIRE</t>
   </si>
   <si>
-    <t>Fonction generique avec la 1ere fonction de recuperation IF id present 
-REFLEXION AVEC UNE FONCTION GLOBALE DE REQUETE</t>
-  </si>
-  <si>
-    <t>la fonction doit ajouter la personnalisation dans le html</t>
-  </si>
-  <si>
     <t>listeProduitsAccueil</t>
   </si>
   <si>
@@ -487,15 +474,42 @@
     <t>POUR CHAQUE index present dans le tableau, AJOUTER les parametres a la fonction creationBlocHTMLAccueil</t>
   </si>
   <si>
-    <t>insertionDescriptifProduits</t>
-  </si>
-  <si>
     <t>accueil js
 porduit js</t>
   </si>
   <si>
     <t>Creation de la fonction promesse qui prend en parametre l'URL et retourne la promesse
 pour la page produit, ajout d'un parametre à l'URL</t>
+  </si>
+  <si>
+    <t>Devtool: inspect l'élément parent pour vérifier comment le bloc HTML est indenté</t>
+  </si>
+  <si>
+    <t>Faire le test avec différents donnees dans le tableau et vérifier si chaque données correspondent bien aux éléments incrémentés dans le HTML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consol.log de getPromise afin de voir si la promesse est bien envoyer et verifier son statuts </t>
+  </si>
+  <si>
+    <t>consol.log du paramètre avec le paramètre de la fonction pour vérifier si les données de la promesse sont bien récupérer</t>
+  </si>
+  <si>
+    <t>La fonction doit créer un nouvel omglet HTML du menu déroulant de personnalisation</t>
+  </si>
+  <si>
+    <t>menuPresonnalisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la fonction récupère les données en paramètre et créer pour chaque index l'onglet du menu déroulant </t>
+  </si>
+  <si>
+    <t>si le tableau de données n'a pas de données ou n'existe alors renvoie une erreur et désactive le bouton</t>
+  </si>
+  <si>
+    <t>nouvelOngletPersonnalisation</t>
+  </si>
+  <si>
+    <t>descriptifProduit</t>
   </si>
 </sst>
 </file>
@@ -944,7 +958,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -999,58 +1013,62 @@
     </row>
     <row r="2" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
         <v>74</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" s="6"/>
+        <v>105</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>118</v>
+      </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" s="6"/>
+        <v>108</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>119</v>
+      </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1059,12 +1077,14 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1073,12 +1093,14 @@
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E7" s="4"/>
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1087,12 +1109,14 @@
       </c>
       <c r="B8" s="22"/>
       <c r="C8" s="14" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E8" s="4"/>
+        <v>110</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1101,41 +1125,45 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="14" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="12"/>
+        <v>103</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="17" t="s">
         <v>76</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>104</v>
+        <v>124</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="17" t="s">
         <v>76</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="14" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="F11" s="4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -1143,10 +1171,10 @@
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -1160,7 +1188,7 @@
         <v>78</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1216,7 +1244,7 @@
         <v>92</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -1241,10 +1269,10 @@
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="12"/>

</xml_diff>

<commit_message>
test de l'evenement au click de envoyer
</commit_message>
<xml_diff>
--- a/Projet/Template+de+Plan+de+tests.xlsx
+++ b/Projet/Template+de+Plan+de+tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggira\Desktop\site\lab\Orinoco\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DAA907-1322-4144-A03B-FB60DE0D5A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0324B9B2-ABA4-4822-B0CE-CE6B6EA8DBBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="142">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -505,6 +505,19 @@
 Ecouter le bouton "submit" au click
 Si la réponse est true alors récuperer la valeur de chaque champs et les envoyer comme paramètre de la fonction objetContactEnvoie
 Sinon ne pas envoyer le formulaire</t>
+  </si>
+  <si>
+    <t>envoieDonneesAPI</t>
+  </si>
+  <si>
+    <t>Simuler les différentes possibilités de validation :
+Si le panier et le formulaire sont vides
+Si seul le panier est vide
+Si seul le formulaire est vide
+Si les 2 sont correctement remplis</t>
+  </si>
+  <si>
+    <t>le panier ne correspond pas a la mise en cache</t>
   </si>
 </sst>
 </file>
@@ -943,9 +956,9 @@
   </sheetPr>
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -954,7 +967,7 @@
     <col min="2" max="2" width="27.140625" customWidth="1"/>
     <col min="3" max="3" width="29.5703125" customWidth="1"/>
     <col min="4" max="4" width="50.5703125" style="23" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="47.28515625" customWidth="1"/>
     <col min="6" max="6" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1156,7 +1169,9 @@
       <c r="E11" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
@@ -1330,13 +1345,19 @@
       <c r="E21" s="4"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="11"/>
-      <c r="C22" s="14"/>
+      <c r="C22" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="D22" s="21"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="E22" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>

</xml_diff>

<commit_message>
ajustement fonction envoie de donnees
</commit_message>
<xml_diff>
--- a/Projet/Template+de+Plan+de+tests.xlsx
+++ b/Projet/Template+de+Plan+de+tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggira\Desktop\site\lab\Orinoco\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0324B9B2-ABA4-4822-B0CE-CE6B6EA8DBBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA421F57-3C98-49D9-B3D4-689686802078}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="148">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -318,9 +318,6 @@
 porduit js</t>
   </si>
   <si>
-    <t>Devtool: inspect l'élément parent pour vérifier comment le bloc HTML est indenté</t>
-  </si>
-  <si>
     <t>Faire le test avec différents donnees dans le tableau et vérifier si chaque données correspondent bien aux éléments incrémentés dans le HTML</t>
   </si>
   <si>
@@ -498,26 +495,53 @@
     <t>Passer les donnees en parametre de la fonction et console.log(mycontact) pour vérifier que l'objet contact est correctement creer</t>
   </si>
   <si>
-    <t>recuperationDonneesContact</t>
-  </si>
-  <si>
-    <t>Recuperer les reponses des fontions controleFormulaire et controleFormulaireEmail
+    <t>envoieDonneesAPI</t>
+  </si>
+  <si>
+    <t>Recuperer les reponses les fonctions controleFormulaire et controleFormulaireEmail
 Ecouter le bouton "submit" au click
 Si la réponse est true alors récuperer la valeur de chaque champs et les envoyer comme paramètre de la fonction objetContactEnvoie
 Sinon ne pas envoyer le formulaire</t>
-  </si>
-  <si>
-    <t>envoieDonneesAPI</t>
   </si>
   <si>
     <t>Simuler les différentes possibilités de validation :
 Si le panier et le formulaire sont vides
 Si seul le panier est vide
 Si seul le formulaire est vide
+Si un seul champs du formulaire est rempli
 Si les 2 sont correctement remplis</t>
   </si>
   <si>
-    <t>le panier ne correspond pas a la mise en cache</t>
+    <t>le panier ne correspond pas a la mise en cache
+la recuperation de la valeur du champs est erronée</t>
+  </si>
+  <si>
+    <t>Envoyer en POST les données converti en objet json.
+Renvoie une promesse si la réponse est ok 
+Sinon envoie une alerte erreur</t>
+  </si>
+  <si>
+    <t>recuperationDonneesEtContact</t>
+  </si>
+  <si>
+    <t>Saisir une URL: 
+-Correcte, console.log pour vérifier la réponse
+-Incorrecte: voir si l'alert windows est bien retourné</t>
+  </si>
+  <si>
+    <t>Inspecter l'élément parent pour vérifier comment le bloc HTML est correctement ajouter</t>
+  </si>
+  <si>
+    <t>Cliquer sur chaque produit et ouvrir le menu déroulant pour vérifier que la personnalisation correspond au produit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le bloc ne se créée pas </t>
+  </si>
+  <si>
+    <t>Ne retourne pas la nombre de quantités totales</t>
+  </si>
+  <si>
+    <t>Le contenu du produit ne s'affiche pas</t>
   </si>
 </sst>
 </file>
@@ -957,8 +981,8 @@
   <dimension ref="A1:Z1009"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1020,11 +1044,13 @@
         <v>74</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" s="6"/>
+        <v>133</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>142</v>
+      </c>
       <c r="F2" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1036,12 +1062,14 @@
         <v>82</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" s="6"/>
+        <v>95</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
@@ -1052,12 +1080,14 @@
         <v>80</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="12"/>
+        <v>97</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
@@ -1068,12 +1098,14 @@
         <v>81</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="12"/>
+        <v>96</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
@@ -1081,15 +1113,17 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="12"/>
+        <v>98</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
@@ -1097,14 +1131,16 @@
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="E7" s="12"/>
+        <v>132</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>143</v>
+      </c>
       <c r="F7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1113,14 +1149,16 @@
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1129,16 +1167,16 @@
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="E9" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1147,13 +1185,17 @@
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="E10" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
@@ -1161,16 +1203,16 @@
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1179,16 +1221,16 @@
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="E12" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1197,15 +1239,17 @@
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F13" s="12"/>
+      <c r="E13" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -1213,16 +1257,16 @@
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1231,16 +1275,16 @@
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D15" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1249,16 +1293,16 @@
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="D16" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1267,16 +1311,16 @@
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E17" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1288,13 +1332,13 @@
         <v>79</v>
       </c>
       <c r="D18" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1303,16 +1347,16 @@
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="E19" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>128</v>
-      </c>
       <c r="F19" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1321,13 +1365,13 @@
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D20" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>135</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="F20" s="12"/>
     </row>
@@ -1337,27 +1381,31 @@
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="E21" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="11"/>
       <c r="C22" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>141</v>
-      </c>
+      <c r="E22" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>

</xml_diff>

<commit_message>
correction validator css color L12
</commit_message>
<xml_diff>
--- a/Projet/Template+de+Plan+de+tests.xlsx
+++ b/Projet/Template+de+Plan+de+tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggira\Desktop\site\lab\Orinoco\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA421F57-3C98-49D9-B3D4-689686802078}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF3CA11-DA11-40E0-91A4-132ED50D4369}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -980,9 +980,9 @@
   </sheetPr>
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>